<commit_message>
Updates to passing network Excel spreadsheets
</commit_message>
<xml_diff>
--- a/stats/passing-networks/nwsl-2016/hou_2016_pass_network.xlsx
+++ b/stats/passing-networks/nwsl-2016/hou_2016_pass_network.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/wosostats/stats/passing-networks/nwsl-2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="19760" windowHeight="8760" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="24520" windowHeight="13700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="passes" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,8 +134,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,8 +180,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -261,16 +274,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3"/>
@@ -298,14 +327,19 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="6" applyAlignment="1">
+      <alignment textRotation="135"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
     <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="6" builtinId="21"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -593,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4083,11 +4117,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="14" max="16" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
@@ -5281,7 +5318,7 @@
         <v>1.3278688524590165</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -5377,7 +5414,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -5473,7 +5510,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -6357,7 +6394,7 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6367,71 +6404,71 @@
     <col min="17" max="24" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
+    <row r="1" spans="1:24" ht="53" x14ac:dyDescent="0.2">
+      <c r="C1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="K1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="28" t="s">
         <v>20</v>
       </c>
     </row>
@@ -6504,7 +6541,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="27" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -6600,7 +6637,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="27" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -6696,7 +6733,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -6792,7 +6829,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="27" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -6888,7 +6925,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="27" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -6984,7 +7021,7 @@
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="27" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -7080,7 +7117,7 @@
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="27" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -7176,7 +7213,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="27" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -7272,7 +7309,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -7368,7 +7405,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="27" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -7464,7 +7501,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="27" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -7560,7 +7597,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -7656,7 +7693,7 @@
       </c>
     </row>
     <row r="15" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="27" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -7752,7 +7789,7 @@
       </c>
     </row>
     <row r="16" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="27" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -7848,7 +7885,7 @@
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="27" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -7944,7 +7981,7 @@
       </c>
     </row>
     <row r="18" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="27" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -8040,7 +8077,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="27" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -8136,7 +8173,7 @@
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -8232,7 +8269,7 @@
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="27" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -8328,7 +8365,7 @@
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="27" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -8424,7 +8461,7 @@
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -8520,7 +8557,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -8637,7 +8674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>

</xml_diff>